<commit_message>
Unneeded review points and revert changes.
</commit_message>
<xml_diff>
--- a/input Documant/cr/Review/PO_SB_CR_WEB_Review.xlsx
+++ b/input Documant/cr/Review/PO_SB_CR_WEB_Review.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Graduation_Project\Web_SWProcess_Documents\input Documant\cr\Review\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mentorship\SB\Web_SWProcess_Documents\Input Documant\CR\Review\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C7CB1B7-571E-4FB5-B912-38A93C9F4476}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
   <si>
     <t>Entry Date</t>
   </si>
@@ -44,33 +43,6 @@
   </si>
   <si>
     <t>Proposed Solution</t>
-  </si>
-  <si>
-    <t>Ahmed Mohamed</t>
-  </si>
-  <si>
-    <t>V1.0</t>
-  </si>
-  <si>
-    <t>2 / / Key Elements/ 4</t>
-  </si>
-  <si>
-    <t>add the point</t>
-  </si>
-  <si>
-    <t xml:space="preserve">	The Customer can see the bumps he met</t>
-  </si>
-  <si>
-    <t>4/ /Mapping Requirements ID’s/ 4</t>
-  </si>
-  <si>
-    <t>The Customer can see the bumps he met</t>
-  </si>
-  <si>
-    <t>CR_REV_0001</t>
-  </si>
-  <si>
-    <t>CR_REV_0002</t>
   </si>
   <si>
     <t>CR_REV_ID</t>
@@ -79,7 +51,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d"/>
   </numFmts>
@@ -182,7 +154,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="عادي" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -418,29 +390,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="1" max="1" width="17.88671875" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="4" max="4" width="32.28515625" customWidth="1"/>
-    <col min="5" max="5" width="35.7109375" customWidth="1"/>
-    <col min="6" max="7" width="44.5703125" customWidth="1"/>
-    <col min="8" max="8" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="32.33203125" customWidth="1"/>
+    <col min="5" max="5" width="35.6640625" customWidth="1"/>
+    <col min="6" max="7" width="44.5546875" customWidth="1"/>
+    <col min="8" max="8" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -464,71 +436,43 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="3">
-        <v>44857</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>12</v>
-      </c>
+    <row r="2" spans="1:8" ht="14.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
       <c r="H2" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="3">
-        <v>44857</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>14</v>
-      </c>
+    <row r="3" spans="1:8" ht="14.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
       <c r="H3" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
+    <row r="4" spans="1:8" ht="14.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2"/>
       <c r="B4" s="3"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
       <c r="H4" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="14.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="3"/>
       <c r="C5" s="2"/>
@@ -540,7 +484,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="3"/>
       <c r="C6" s="2"/>
@@ -552,7 +496,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="3"/>
       <c r="C7" s="2"/>
@@ -564,44 +508,20 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <conditionalFormatting sqref="A2:H9">
+  <conditionalFormatting sqref="A2:H7">
     <cfRule type="expression" dxfId="1" priority="3">
       <formula>$H2 = "Closed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:H9">
+  <conditionalFormatting sqref="A2:H7">
     <cfRule type="expression" dxfId="0" priority="4">
       <formula>$H2= "Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Open" sqref="H2:H9" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Open" sqref="H2:H7">
       <formula1>"Open,Closed"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>